<commit_message>
Reverse a linked list Iterative
Reverse a linked list Iterative
</commit_message>
<xml_diff>
--- a/Learning points/FINAL450.xlsx
+++ b/Learning points/FINAL450.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://atos365-my.sharepoint.com/personal/abhishek_rahul_atos_net/Documents/Desktop/Personal/Abhishek/Interview/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://atos365-my.sharepoint.com/personal/abhishek_rahul_atos_net/Documents/Desktop/Personal/practice/DataStructure/Learning points/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="9" documentId="8_{A296DB3B-D750-F440-AE8C-C019300B98C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AA64049-BD30-4F87-988C-B04E1EA3A7B4}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView minimized="1" xWindow="3480" yWindow="2840" windowWidth="14400" windowHeight="7360" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1858,8 +1858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView topLeftCell="A151" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="A139" sqref="A139:C174"/>
+    <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -7386,7 +7386,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F94E04F-3288-489D-976B-C5CC42FB1945}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
reverse kth in group
</commit_message>
<xml_diff>
--- a/Learning points/FINAL450.xlsx
+++ b/Learning points/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://atos365-my.sharepoint.com/personal/abhishek_rahul_atos_net/Documents/Desktop/Personal/practice/DataStructure/Learning points/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{A296DB3B-D750-F440-AE8C-C019300B98C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F98AEB0-78B4-43CE-8249-A951BE200263}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{A296DB3B-D750-F440-AE8C-C019300B98C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6664D3A8-CDCD-429E-A823-75FCD3A74494}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,8 +1861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="E150" sqref="E150"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
+      <selection activeCell="C141" sqref="C141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3319,7 +3319,7 @@
         <v>136</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Check if a linked list is a circular linked list.
</commit_message>
<xml_diff>
--- a/Learning points/FINAL450.xlsx
+++ b/Learning points/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://atos365-my.sharepoint.com/personal/abhishek_rahul_atos_net/Documents/Desktop/Personal/practice/DataStructure/Learning points/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{A296DB3B-D750-F440-AE8C-C019300B98C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6664D3A8-CDCD-429E-A823-75FCD3A74494}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{A296DB3B-D750-F440-AE8C-C019300B98C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7D97080-DA60-4624-9DA4-6E2BB8A8FD8B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,8 +1861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="C141" sqref="C141"/>
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
+      <selection activeCell="D153" sqref="D153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3473,7 +3473,7 @@
         <v>150</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="21">

</xml_diff>

<commit_message>
List list code changes
</commit_message>
<xml_diff>
--- a/Learning points/FINAL450.xlsx
+++ b/Learning points/FINAL450.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://atos365-my.sharepoint.com/personal/abhishek_rahul_atos_net/Documents/Desktop/Personal/practice/DataStructure/Learning points/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{A296DB3B-D750-F440-AE8C-C019300B98C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7D97080-DA60-4624-9DA4-6E2BB8A8FD8B}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{A296DB3B-D750-F440-AE8C-C019300B98C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AE264FA-05B6-422B-9F8F-2B02F05E67EC}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView minimized="1" xWindow="3480" yWindow="2840" windowWidth="14400" windowHeight="7360" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="467">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1430,6 +1431,9 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>wip</t>
   </si>
 </sst>
 </file>
@@ -1861,8 +1865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="D153" sqref="D153"/>
+    <sheetView tabSelected="1" topLeftCell="A153" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
+      <selection activeCell="C172" sqref="C172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3330,7 +3334,7 @@
         <v>137</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="21">
@@ -3341,7 +3345,7 @@
         <v>138</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="21">
@@ -3352,7 +3356,7 @@
         <v>139</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="21">
@@ -3363,7 +3367,7 @@
         <v>140</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="21">
@@ -3374,7 +3378,7 @@
         <v>141</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="21">
@@ -3616,7 +3620,7 @@
         <v>163</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>4</v>
+        <v>466</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Merge K sorted Linked list
</commit_message>
<xml_diff>
--- a/Learning points/FINAL450.xlsx
+++ b/Learning points/FINAL450.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://atos365-my.sharepoint.com/personal/abhishek_rahul_atos_net/Documents/Desktop/Personal/practice/DataStructure/Learning points/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{A296DB3B-D750-F440-AE8C-C019300B98C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AE264FA-05B6-422B-9F8F-2B02F05E67EC}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{A296DB3B-D750-F440-AE8C-C019300B98C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49955884-9773-4D6B-9A76-51DB03F65EEF}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3480" yWindow="2840" windowWidth="14400" windowHeight="7360" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="466">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1431,9 +1430,6 @@
   </si>
   <si>
     <t>yes</t>
-  </si>
-  <si>
-    <t>wip</t>
   </si>
 </sst>
 </file>
@@ -1865,8 +1861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A153" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="C172" sqref="C172"/>
+    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
+      <selection activeCell="E168" sqref="E168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3620,7 +3616,7 @@
         <v>163</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="21">
@@ -3642,7 +3638,7 @@
         <v>165</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="21">

</xml_diff>